<commit_message>
Ready to PCB edit.
</commit_message>
<xml_diff>
--- a/DCマウス2016_部品表.xlsx
+++ b/DCマウス2016_部品表.xlsx
@@ -1204,41 +1204,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>東北マウス赫で使ったのと同じもの
-RTで見積もりしてもらう必要あり。以前聞いた話だとたしか単価5000くらい</t>
-    <rPh sb="0" eb="2">
-      <t>トウホク</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>カク</t>
-    </rPh>
-    <rPh sb="7" eb="8">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="12" eb="13">
-      <t>オナ</t>
-    </rPh>
-    <rPh sb="20" eb="22">
-      <t>ミツ</t>
-    </rPh>
-    <rPh sb="29" eb="31">
-      <t>ヒツヨウ</t>
-    </rPh>
-    <rPh sb="34" eb="36">
-      <t>イゼン</t>
-    </rPh>
-    <rPh sb="36" eb="37">
-      <t>キ</t>
-    </rPh>
-    <rPh sb="39" eb="40">
-      <t>ハナシ</t>
-    </rPh>
-    <rPh sb="45" eb="47">
-      <t>タンカ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>磁気エンコーダユニット断面図(案)</t>
     <rPh sb="0" eb="2">
       <t>ジキ</t>
@@ -1407,6 +1372,63 @@
     </rPh>
     <rPh sb="21" eb="23">
       <t>ヘンコウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>東北マウス赫で使ったのと同じもの
+RTで見積もりしてもらう必要あり。以前聞いた話だとたしか単価5000くらい
+→アラオカで見積もりした結果、10個作成で単価約2000円</t>
+    <rPh sb="0" eb="2">
+      <t>トウホク</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>カク</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>オナ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>ミツ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="34" eb="36">
+      <t>イゼン</t>
+    </rPh>
+    <rPh sb="36" eb="37">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="39" eb="40">
+      <t>ハナシ</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>タンカ</t>
+    </rPh>
+    <rPh sb="61" eb="63">
+      <t>ミツ</t>
+    </rPh>
+    <rPh sb="67" eb="69">
+      <t>ケッカ</t>
+    </rPh>
+    <rPh sb="72" eb="73">
+      <t>コ</t>
+    </rPh>
+    <rPh sb="73" eb="75">
+      <t>サクセイ</t>
+    </rPh>
+    <rPh sb="76" eb="78">
+      <t>タンカ</t>
+    </rPh>
+    <rPh sb="78" eb="79">
+      <t>ヤク</t>
+    </rPh>
+    <rPh sb="83" eb="84">
+      <t>エン</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -3552,19 +3574,19 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="G1" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H1" s="16">
         <f>F48</f>
-        <v>33335</v>
+        <v>27335</v>
       </c>
       <c r="J1" s="17">
-        <v>42394</v>
+        <v>42455</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="G2" s="15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H2" s="15">
         <v>10</v>
@@ -3572,7 +3594,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="G3" s="15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H3" s="16">
         <f>F51</f>
@@ -3581,11 +3603,11 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="G4" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H4" s="16">
         <f>(H1*H2)+H3</f>
-        <v>338350</v>
+        <v>278350</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
@@ -3660,10 +3682,10 @@
         <v>72</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="27" x14ac:dyDescent="0.15">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A10" s="5">
         <f t="shared" si="1"/>
         <v>3</v>
@@ -3675,17 +3697,17 @@
         <v>2</v>
       </c>
       <c r="E10" s="2">
-        <v>5000</v>
+        <v>2000</v>
       </c>
       <c r="F10" s="2">
         <f>E10*D10</f>
-        <v>10000</v>
+        <v>4000</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>66</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>159</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="27" x14ac:dyDescent="0.15">
@@ -4118,10 +4140,10 @@
         <v>20</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D27" s="1">
         <v>2</v>
@@ -4134,7 +4156,7 @@
         <v>378</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.15">
@@ -4277,7 +4299,7 @@
         <v>24</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D33" s="1">
         <v>7</v>
@@ -4333,7 +4355,7 @@
         <v>50</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D35" s="1">
         <v>4</v>
@@ -4361,7 +4383,7 @@
         <v>50</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D36" s="1">
         <v>4</v>
@@ -4610,7 +4632,7 @@
         <v>38</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D45" s="1">
         <v>2</v>
@@ -4623,10 +4645,10 @@
         <v>1000</v>
       </c>
       <c r="G45" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="H45" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.15">
@@ -4657,10 +4679,10 @@
     <row r="48" spans="1:8" x14ac:dyDescent="0.15">
       <c r="F48" s="13">
         <f>SUM(F8:F46)</f>
-        <v>33335</v>
+        <v>27335</v>
       </c>
       <c r="G48" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.15">
@@ -4688,7 +4710,7 @@
         <v>106</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.15">
@@ -4887,7 +4909,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -5062,7 +5086,7 @@
   <sheetData>
     <row r="1" spans="2:22" x14ac:dyDescent="0.15">
       <c r="C1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="2:22" x14ac:dyDescent="0.15">
@@ -5243,7 +5267,7 @@
         <v>42394</v>
       </c>
       <c r="C3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.15">
@@ -5251,7 +5275,7 @@
         <v>42394</v>
       </c>
       <c r="C4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>